<commit_message>
Done Linear Regression A2 - Analysis
</commit_message>
<xml_diff>
--- a/4-Analysis/Linear Regression/Linear Regression A1-test.xlsx
+++ b/4-Analysis/Linear Regression/Linear Regression A1-test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Linear Regression" sheetId="1" state="visible" r:id="rId2"/>
@@ -357,7 +357,7 @@
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -381,16 +381,10 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="4" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="5" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -401,12 +395,6 @@
     <xf fontId="0" fillId="4" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="5" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="6" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1">
@@ -421,10 +409,6 @@
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -769,7 +753,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>30479</xdr:colOff>
+      <xdr:colOff>30478</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -819,7 +803,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>30479</xdr:colOff>
+      <xdr:colOff>30478</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>175736</xdr:rowOff>
     </xdr:from>
@@ -869,7 +853,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>30479</xdr:colOff>
+      <xdr:colOff>30478</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>173831</xdr:rowOff>
     </xdr:from>
@@ -919,7 +903,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>30479</xdr:colOff>
+      <xdr:colOff>30478</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>4286</xdr:rowOff>
     </xdr:from>
@@ -969,15 +953,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>30479</xdr:colOff>
+      <xdr:colOff>30478</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>179546</xdr:rowOff>
+      <xdr:rowOff>179545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>611500</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>179546</xdr:rowOff>
+      <xdr:rowOff>179545</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1019,7 +1003,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>13334</xdr:colOff>
+      <xdr:colOff>13333</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>178592</xdr:rowOff>
     </xdr:from>
@@ -1069,7 +1053,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>13334</xdr:colOff>
+      <xdr:colOff>13333</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>175735</xdr:rowOff>
     </xdr:from>
@@ -1119,7 +1103,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>13334</xdr:colOff>
+      <xdr:colOff>13333</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>173830</xdr:rowOff>
     </xdr:from>
@@ -1169,7 +1153,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>13334</xdr:colOff>
+      <xdr:colOff>13333</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>4285</xdr:rowOff>
     </xdr:from>
@@ -1219,7 +1203,7 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>13334</xdr:colOff>
+      <xdr:colOff>13333</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>179545</xdr:rowOff>
     </xdr:from>
@@ -1380,7 +1364,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>591021</xdr:colOff>
+      <xdr:colOff>591020</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>173831</xdr:rowOff>
     </xdr:to>
@@ -1430,7 +1414,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>591020</xdr:colOff>
+      <xdr:colOff>591019</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>182879</xdr:rowOff>
     </xdr:to>
@@ -1476,13 +1460,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>9998</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>179546</xdr:rowOff>
+      <xdr:rowOff>179545</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>591019</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>179546</xdr:rowOff>
+      <xdr:rowOff>179545</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -1856,7 +1840,7 @@
   <tableColumns count="1">
     <tableColumn id="1" name="Results "/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1876,7 +1860,7 @@
   <tableColumns count="1">
     <tableColumn id="1" name="Test case 4.0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1946,7 +1930,7 @@
   <tableColumns count="1">
     <tableColumn id="1" name="Results "/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1956,7 +1940,7 @@
   <tableColumns count="1">
     <tableColumn id="1" name="Test case 4.4"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2659,7 +2643,6 @@
         <v>5</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="L3"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6" t="s">
         <v>5</v>
@@ -2682,34 +2665,34 @@
       <c r="E4" s="10">
         <v>74366.377999999997</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="J4" s="10">
         <v>73459.580000000002</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="12">
         <v>73459.646999999997</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" t="s">
         <v>7</v>
       </c>
-      <c r="T4" s="13">
+      <c r="T4" s="12">
         <v>73363.759000000005</v>
       </c>
       <c r="V4" t="s">
@@ -2726,7 +2709,7 @@
       </c>
     </row>
     <row r="5" ht="15.75">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
@@ -2735,37 +2718,37 @@
       <c r="E5" s="10">
         <v>272.702</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="H5" s="6"/>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="11" t="s">
         <v>16</v>
       </c>
       <c r="J5" s="10">
         <v>271.03399999999999</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="12">
         <v>271.03399999999999</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="R5" s="6"/>
       <c r="S5" t="s">
         <v>16</v>
       </c>
-      <c r="T5" s="13">
+      <c r="T5" s="12">
         <v>270.85700000000003</v>
       </c>
-      <c r="V5" s="16">
+      <c r="V5" s="14">
         <v>1</v>
       </c>
       <c r="W5">
@@ -2779,7 +2762,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
@@ -2788,37 +2771,37 @@
       <c r="E6" s="10">
         <v>134.86699999999999</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H6" s="6"/>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="10">
         <v>130.68600000000001</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="13" t="s">
         <v>18</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="12">
         <v>130.68600000000001</v>
       </c>
-      <c r="Q6" s="14" t="s">
+      <c r="Q6" s="13" t="s">
         <v>18</v>
       </c>
       <c r="R6" s="6"/>
       <c r="S6" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="13">
+      <c r="T6" s="12">
         <v>130.572</v>
       </c>
-      <c r="V6" s="16"/>
+      <c r="V6" s="14"/>
     </row>
     <row r="7">
       <c r="D7" t="s">
@@ -2828,7 +2811,7 @@
         <v>0.89200000000000002</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="11" t="s">
         <v>20</v>
       </c>
       <c r="J7" s="10">
@@ -2839,7 +2822,7 @@
       <c r="N7" t="s">
         <v>20</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="12">
         <v>0.83699999999999997</v>
       </c>
       <c r="Q7" s="6"/>
@@ -2847,7 +2830,7 @@
       <c r="S7" t="s">
         <v>20</v>
       </c>
-      <c r="T7" s="13">
+      <c r="T7" s="12">
         <v>0.83799999999999997</v>
       </c>
       <c r="V7" s="6" t="s">
@@ -2872,7 +2855,7 @@
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="11" t="s">
         <v>21</v>
       </c>
       <c r="J8" s="10">
@@ -2883,7 +2866,7 @@
       <c r="N8" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="12">
         <v>0.68200000000000005</v>
       </c>
       <c r="Q8" s="6"/>
@@ -2891,10 +2874,10 @@
       <c r="S8" t="s">
         <v>21</v>
       </c>
-      <c r="T8" s="13">
+      <c r="T8" s="12">
         <v>0.68200000000000005</v>
       </c>
-      <c r="V8" s="16">
+      <c r="V8" s="14">
         <v>2</v>
       </c>
       <c r="W8" s="6">
@@ -2911,15 +2894,15 @@
       <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="15">
         <v>1.3</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="16">
         <v>1.2</v>
       </c>
       <c r="L9" s="6"/>
@@ -2927,7 +2910,7 @@
       <c r="N9" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="17">
         <v>2.04</v>
       </c>
       <c r="Q9" s="6"/>
@@ -2935,10 +2918,10 @@
       <c r="S9" t="s">
         <v>22</v>
       </c>
-      <c r="T9" s="19">
+      <c r="T9" s="17">
         <v>1.1899999999999999</v>
       </c>
-      <c r="V9" s="16">
+      <c r="V9" s="14">
         <v>2.1000000000000001</v>
       </c>
       <c r="W9" s="6">
@@ -2954,27 +2937,26 @@
     <row r="10">
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
-      <c r="N10" s="20"/>
+      <c r="N10" s="18"/>
       <c r="O10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
-      <c r="S10" s="20"/>
+      <c r="S10" s="18"/>
       <c r="T10" s="6"/>
-      <c r="V10" s="21">
+      <c r="V10" s="14">
         <v>2.2000000000000002</v>
       </c>
-      <c r="W10" s="22">
+      <c r="W10" s="6">
         <v>68</v>
       </c>
-      <c r="X10" s="22">
+      <c r="X10" s="6">
         <v>1.2</v>
       </c>
-      <c r="Y10" s="22">
+      <c r="Y10" s="6">
         <v>0.82999999999999996</v>
       </c>
     </row>
     <row r="11" ht="15.75">
-      <c r="G11"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
         <v>5</v>
@@ -2992,7 +2974,7 @@
         <v>5</v>
       </c>
       <c r="T11" s="8"/>
-      <c r="V11" s="16">
+      <c r="V11" s="14">
         <v>2.2999999999999998</v>
       </c>
       <c r="W11" s="6">
@@ -3006,75 +2988,75 @@
       </c>
     </row>
     <row r="12" ht="15.75">
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H12" s="6"/>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="19" t="s">
         <v>7</v>
       </c>
       <c r="J12" s="10">
         <v>73459.354000000007</v>
       </c>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="6" t="s">
         <v>24</v>
       </c>
       <c r="M12" s="6"/>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="19" t="s">
         <v>7</v>
       </c>
       <c r="O12" s="10">
         <v>73459.514999999999</v>
       </c>
-      <c r="Q12" s="11" t="s">
+      <c r="Q12" s="6" t="s">
         <v>25</v>
       </c>
       <c r="R12" s="6"/>
-      <c r="S12" s="23" t="s">
+      <c r="S12" s="19" t="s">
         <v>7</v>
       </c>
       <c r="T12" s="10">
         <v>73279.675000000003</v>
       </c>
-      <c r="V12" s="24">
+      <c r="V12" s="20">
         <v>2.3999999999999999</v>
       </c>
-      <c r="W12" s="25">
+      <c r="W12" s="21">
         <v>68</v>
       </c>
-      <c r="X12" s="25">
+      <c r="X12" s="21">
         <v>1.1699999999999999</v>
       </c>
-      <c r="Y12" s="25">
+      <c r="Y12" s="21">
         <v>0.84999999999999998</v>
       </c>
     </row>
     <row r="13">
-      <c r="G13" s="26" t="s">
+      <c r="G13" s="22" t="s">
         <v>26</v>
       </c>
       <c r="H13" s="6"/>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="23" t="s">
         <v>16</v>
       </c>
       <c r="J13" s="10">
         <v>271.03399999999999</v>
       </c>
-      <c r="L13" s="26" t="s">
+      <c r="L13" s="22" t="s">
         <v>26</v>
       </c>
       <c r="M13" s="6"/>
-      <c r="N13" s="27" t="s">
+      <c r="N13" s="23" t="s">
         <v>16</v>
       </c>
       <c r="O13" s="10">
         <v>271.03399999999999</v>
       </c>
-      <c r="Q13" s="26" t="s">
+      <c r="Q13" s="22" t="s">
         <v>26</v>
       </c>
       <c r="R13" s="6"/>
-      <c r="S13" s="27" t="s">
+      <c r="S13" s="23" t="s">
         <v>16</v>
       </c>
       <c r="T13" s="10">
@@ -3082,31 +3064,31 @@
       </c>
     </row>
     <row r="14">
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H14" s="6"/>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="10">
         <v>130.68600000000001</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="13" t="s">
         <v>18</v>
       </c>
       <c r="M14" s="6"/>
-      <c r="N14" s="23" t="s">
+      <c r="N14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="O14" s="10">
         <v>130.68600000000001</v>
       </c>
-      <c r="Q14" s="15" t="s">
+      <c r="Q14" s="13" t="s">
         <v>18</v>
       </c>
       <c r="R14" s="6"/>
-      <c r="S14" s="23" t="s">
+      <c r="S14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="T14" s="10">
@@ -3128,7 +3110,7 @@
     <row r="15">
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="23" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="10">
@@ -3136,7 +3118,7 @@
       </c>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="27" t="s">
+      <c r="N15" s="23" t="s">
         <v>20</v>
       </c>
       <c r="O15" s="10">
@@ -3144,29 +3126,29 @@
       </c>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
-      <c r="S15" s="27" t="s">
+      <c r="S15" s="23" t="s">
         <v>20</v>
       </c>
       <c r="T15" s="10">
         <v>0.83799999999999997</v>
       </c>
-      <c r="V15" s="24">
+      <c r="V15" s="20">
         <v>3</v>
       </c>
-      <c r="W15" s="25">
+      <c r="W15" s="21">
         <v>68</v>
       </c>
-      <c r="X15" s="25">
+      <c r="X15" s="21">
         <v>2.04</v>
       </c>
-      <c r="Y15" s="25">
+      <c r="Y15" s="21">
         <v>0.48999999999999999</v>
       </c>
     </row>
     <row r="16">
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="19" t="s">
         <v>21</v>
       </c>
       <c r="J16" s="10">
@@ -3174,7 +3156,7 @@
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="23" t="s">
+      <c r="N16" s="19" t="s">
         <v>21</v>
       </c>
       <c r="O16" s="10">
@@ -3182,13 +3164,13 @@
       </c>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="23" t="s">
+      <c r="S16" s="19" t="s">
         <v>21</v>
       </c>
       <c r="T16" s="10">
         <v>0.68200000000000005</v>
       </c>
-      <c r="V16" s="16">
+      <c r="V16" s="14">
         <v>3.1000000000000001</v>
       </c>
       <c r="W16" s="6">
@@ -3204,51 +3186,51 @@
     <row r="17">
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="16">
         <v>1.2</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="27" t="s">
+      <c r="N17" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="O17" s="18">
+      <c r="O17" s="16">
         <v>2.0800000000000001</v>
       </c>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="S17" s="27" t="s">
+      <c r="S17" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="T17" s="18">
+      <c r="T17" s="16">
         <v>2.1000000000000001</v>
       </c>
-      <c r="V17" s="21">
+      <c r="V17" s="14">
         <v>3.2000000000000002</v>
       </c>
-      <c r="W17" s="22">
+      <c r="W17" s="6">
         <v>68</v>
       </c>
-      <c r="X17" s="22">
+      <c r="X17" s="6">
         <v>2.0800000000000001</v>
       </c>
-      <c r="Y17" s="22">
+      <c r="Y17" s="6">
         <v>0.47999999999999998</v>
       </c>
     </row>
     <row r="18">
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="20"/>
+      <c r="N18" s="18"/>
       <c r="O18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
-      <c r="S18" s="20"/>
+      <c r="S18" s="18"/>
       <c r="T18" s="6"/>
-      <c r="V18" s="16">
+      <c r="V18" s="14">
         <v>3.2999999999999998</v>
       </c>
       <c r="W18" s="6">
@@ -3262,8 +3244,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="15"/>
-      <c r="G19"/>
+      <c r="B19" s="13"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6" t="s">
         <v>5</v>
@@ -3281,7 +3262,7 @@
         <v>5</v>
       </c>
       <c r="T19" s="8"/>
-      <c r="V19" s="16">
+      <c r="V19" s="14">
         <v>3.3999999999999999</v>
       </c>
       <c r="W19" s="6">
@@ -3295,32 +3276,32 @@
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="15"/>
-      <c r="G20" s="11" t="s">
+      <c r="B20" s="13"/>
+      <c r="G20" s="6" t="s">
         <v>27</v>
       </c>
       <c r="H20" s="6"/>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="19" t="s">
         <v>7</v>
       </c>
       <c r="J20" s="10">
         <v>73459.126999999993</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="6" t="s">
         <v>28</v>
       </c>
       <c r="M20" s="6"/>
-      <c r="N20" s="23" t="s">
+      <c r="N20" s="19" t="s">
         <v>7</v>
       </c>
       <c r="O20" s="10">
         <v>73459.445999999996</v>
       </c>
-      <c r="Q20" s="11" t="s">
+      <c r="Q20" s="6" t="s">
         <v>29</v>
       </c>
       <c r="R20" s="6"/>
-      <c r="S20" s="23" t="s">
+      <c r="S20" s="19" t="s">
         <v>7</v>
       </c>
       <c r="T20" s="10">
@@ -3328,31 +3309,31 @@
       </c>
     </row>
     <row r="21">
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="22" t="s">
         <v>30</v>
       </c>
       <c r="H21" s="6"/>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="23" t="s">
         <v>16</v>
       </c>
       <c r="J21" s="10">
         <v>271.03300000000002</v>
       </c>
-      <c r="L21" s="26" t="s">
+      <c r="L21" s="22" t="s">
         <v>30</v>
       </c>
       <c r="M21" s="6"/>
-      <c r="N21" s="27" t="s">
+      <c r="N21" s="23" t="s">
         <v>16</v>
       </c>
       <c r="O21" s="10">
         <v>271.03399999999999</v>
       </c>
-      <c r="Q21" s="26" t="s">
+      <c r="Q21" s="22" t="s">
         <v>30</v>
       </c>
       <c r="R21" s="6"/>
-      <c r="S21" s="27" t="s">
+      <c r="S21" s="23" t="s">
         <v>16</v>
       </c>
       <c r="T21" s="10">
@@ -3372,53 +3353,53 @@
       </c>
     </row>
     <row r="22">
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H22" s="6"/>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="19" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="10">
         <v>130.68600000000001</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="L22" s="13" t="s">
         <v>18</v>
       </c>
       <c r="M22" s="6"/>
-      <c r="N22" s="23" t="s">
+      <c r="N22" s="19" t="s">
         <v>19</v>
       </c>
       <c r="O22" s="10">
         <v>130.68600000000001</v>
       </c>
-      <c r="Q22" s="15" t="s">
+      <c r="Q22" s="13" t="s">
         <v>18</v>
       </c>
       <c r="R22" s="6"/>
-      <c r="S22" s="23" t="s">
+      <c r="S22" s="19" t="s">
         <v>19</v>
       </c>
       <c r="T22" s="10">
         <v>130.381</v>
       </c>
-      <c r="V22" s="24">
+      <c r="V22" s="20">
         <v>4</v>
       </c>
-      <c r="W22" s="25">
+      <c r="W22" s="21">
         <v>68</v>
       </c>
-      <c r="X22" s="25">
+      <c r="X22" s="21">
         <v>1.1899999999999999</v>
       </c>
-      <c r="Y22" s="25">
+      <c r="Y22" s="21">
         <v>0.83999999999999997</v>
       </c>
     </row>
     <row r="23">
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="27" t="s">
+      <c r="I23" s="23" t="s">
         <v>20</v>
       </c>
       <c r="J23" s="10">
@@ -3426,7 +3407,7 @@
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
-      <c r="N23" s="27" t="s">
+      <c r="N23" s="23" t="s">
         <v>20</v>
       </c>
       <c r="O23" s="10">
@@ -3434,13 +3415,13 @@
       </c>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
-      <c r="S23" s="27" t="s">
+      <c r="S23" s="23" t="s">
         <v>20</v>
       </c>
       <c r="T23" s="10">
         <v>0.83999999999999997</v>
       </c>
-      <c r="V23" s="16">
+      <c r="V23" s="14">
         <v>4.0999999999999996</v>
       </c>
       <c r="W23" s="6">
@@ -3456,7 +3437,7 @@
     <row r="24">
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="19" t="s">
         <v>21</v>
       </c>
       <c r="J24" s="10">
@@ -3464,7 +3445,7 @@
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-      <c r="N24" s="23" t="s">
+      <c r="N24" s="19" t="s">
         <v>21</v>
       </c>
       <c r="O24" s="10">
@@ -3472,52 +3453,52 @@
       </c>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
-      <c r="S24" s="23" t="s">
+      <c r="S24" s="19" t="s">
         <v>21</v>
       </c>
       <c r="T24" s="10">
         <v>0.68300000000000005</v>
       </c>
-      <c r="V24" s="21">
+      <c r="V24" s="14">
         <v>4.2000000000000002</v>
       </c>
-      <c r="W24" s="22">
+      <c r="W24" s="6">
         <v>68</v>
       </c>
-      <c r="X24" s="22">
+      <c r="X24" s="6">
         <v>1.8999999999999999</v>
       </c>
-      <c r="Y24" s="22">
+      <c r="Y24" s="6">
         <v>0.52000000000000002</v>
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="15"/>
+      <c r="B25" s="13"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="18">
+      <c r="J25" s="16">
         <v>1.2</v>
       </c>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
-      <c r="N25" s="27" t="s">
+      <c r="N25" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="18">
+      <c r="O25" s="16">
         <v>2.0800000000000001</v>
       </c>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
-      <c r="S25" s="27" t="s">
+      <c r="S25" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="T25" s="18">
+      <c r="T25" s="16">
         <v>1.8999999999999999</v>
       </c>
-      <c r="V25" s="16">
+      <c r="V25" s="14">
         <v>4.2999999999999998</v>
       </c>
       <c r="W25" s="6">
@@ -3531,20 +3512,20 @@
       </c>
     </row>
     <row r="26" ht="15.75">
-      <c r="B26" s="15"/>
+      <c r="B26" s="13"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="20"/>
+      <c r="I26" s="18"/>
       <c r="J26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
-      <c r="N26" s="20"/>
+      <c r="N26" s="18"/>
       <c r="O26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="20"/>
+      <c r="S26" s="18"/>
       <c r="T26" s="6"/>
-      <c r="V26" s="16">
+      <c r="V26" s="14">
         <v>4.4000000000000004</v>
       </c>
       <c r="W26" s="6">
@@ -3558,7 +3539,7 @@
       </c>
     </row>
     <row r="27" ht="15.75">
-      <c r="B27" s="15"/>
+      <c r="B27" s="13"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="9" t="s">
@@ -3579,32 +3560,32 @@
       <c r="T27" s="8"/>
     </row>
     <row r="28">
-      <c r="B28" s="15"/>
-      <c r="G28" s="11" t="s">
+      <c r="B28" s="13"/>
+      <c r="G28" s="6" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="6"/>
-      <c r="I28" s="23" t="s">
+      <c r="I28" s="19" t="s">
         <v>7</v>
       </c>
       <c r="J28" s="10">
         <v>73458.900999999998</v>
       </c>
-      <c r="L28" s="11" t="s">
+      <c r="L28" s="6" t="s">
         <v>32</v>
       </c>
       <c r="M28" s="6"/>
-      <c r="N28" s="23" t="s">
+      <c r="N28" s="19" t="s">
         <v>7</v>
       </c>
       <c r="O28" s="10">
         <v>73459.346000000005</v>
       </c>
-      <c r="Q28" s="11" t="s">
+      <c r="Q28" s="6" t="s">
         <v>33</v>
       </c>
       <c r="R28" s="6"/>
-      <c r="S28" s="23" t="s">
+      <c r="S28" s="19" t="s">
         <v>7</v>
       </c>
       <c r="T28" s="10">
@@ -3612,31 +3593,31 @@
       </c>
     </row>
     <row r="29">
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="22" t="s">
         <v>34</v>
       </c>
       <c r="H29" s="6"/>
-      <c r="I29" s="27" t="s">
+      <c r="I29" s="23" t="s">
         <v>16</v>
       </c>
       <c r="J29" s="10">
         <v>271.03300000000002</v>
       </c>
-      <c r="L29" s="26" t="s">
+      <c r="L29" s="22" t="s">
         <v>34</v>
       </c>
       <c r="M29" s="6"/>
-      <c r="N29" s="27" t="s">
+      <c r="N29" s="23" t="s">
         <v>16</v>
       </c>
       <c r="O29" s="10">
         <v>271.03399999999999</v>
       </c>
-      <c r="Q29" s="26" t="s">
+      <c r="Q29" s="22" t="s">
         <v>34</v>
       </c>
       <c r="R29" s="6"/>
-      <c r="S29" s="27" t="s">
+      <c r="S29" s="23" t="s">
         <v>16</v>
       </c>
       <c r="T29" s="10">
@@ -3644,31 +3625,31 @@
       </c>
     </row>
     <row r="30">
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H30" s="6"/>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="19" t="s">
         <v>19</v>
       </c>
       <c r="J30" s="10">
         <v>130.685</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="13" t="s">
         <v>18</v>
       </c>
       <c r="M30" s="6"/>
-      <c r="N30" s="23" t="s">
+      <c r="N30" s="19" t="s">
         <v>19</v>
       </c>
       <c r="O30" s="10">
         <v>130.68600000000001</v>
       </c>
-      <c r="Q30" s="15" t="s">
+      <c r="Q30" s="13" t="s">
         <v>18</v>
       </c>
       <c r="R30" s="6"/>
-      <c r="S30" s="23" t="s">
+      <c r="S30" s="19" t="s">
         <v>19</v>
       </c>
       <c r="T30" s="10">
@@ -3678,7 +3659,7 @@
     <row r="31">
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
-      <c r="I31" s="27" t="s">
+      <c r="I31" s="23" t="s">
         <v>20</v>
       </c>
       <c r="J31" s="10">
@@ -3686,7 +3667,7 @@
       </c>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="27" t="s">
+      <c r="N31" s="23" t="s">
         <v>20</v>
       </c>
       <c r="O31" s="10">
@@ -3694,7 +3675,7 @@
       </c>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
-      <c r="S31" s="27" t="s">
+      <c r="S31" s="23" t="s">
         <v>20</v>
       </c>
       <c r="T31" s="10">
@@ -3702,10 +3683,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="15"/>
+      <c r="B32" s="13"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
-      <c r="I32" s="23" t="s">
+      <c r="I32" s="19" t="s">
         <v>21</v>
       </c>
       <c r="J32" s="10">
@@ -3713,7 +3694,7 @@
       </c>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
-      <c r="N32" s="23" t="s">
+      <c r="N32" s="19" t="s">
         <v>21</v>
       </c>
       <c r="O32" s="10">
@@ -3721,7 +3702,7 @@
       </c>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
-      <c r="S32" s="23" t="s">
+      <c r="S32" s="19" t="s">
         <v>21</v>
       </c>
       <c r="T32" s="10">
@@ -3729,49 +3710,49 @@
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="15"/>
+      <c r="B33" s="13"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
-      <c r="I33" s="27" t="s">
+      <c r="I33" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J33" s="18">
+      <c r="J33" s="16">
         <v>1.2</v>
       </c>
       <c r="L33" s="6"/>
       <c r="M33" s="6"/>
-      <c r="N33" s="27" t="s">
+      <c r="N33" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="O33" s="28">
+      <c r="O33" s="16">
         <v>2.2000000000000002</v>
       </c>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
-      <c r="S33" s="27" t="s">
+      <c r="S33" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="T33" s="18">
+      <c r="T33" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="15"/>
+      <c r="B34" s="13"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
-      <c r="N34" s="20"/>
+      <c r="N34" s="18"/>
       <c r="O34" s="6"/>
       <c r="Q34" s="6"/>
       <c r="R34" s="6"/>
-      <c r="S34" s="20"/>
+      <c r="S34" s="18"/>
       <c r="T34" s="6"/>
     </row>
     <row r="35">
-      <c r="B35" s="15"/>
+      <c r="B35" s="13"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="9" t="s">
@@ -3792,31 +3773,31 @@
       <c r="T35" s="8"/>
     </row>
     <row r="36">
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" t="s">
         <v>7</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="12">
         <v>73458.673999999999</v>
       </c>
-      <c r="L36" s="11" t="s">
+      <c r="L36" s="6" t="s">
         <v>36</v>
       </c>
       <c r="M36" s="6"/>
-      <c r="N36" s="23" t="s">
+      <c r="N36" s="19" t="s">
         <v>7</v>
       </c>
       <c r="O36" s="10">
         <v>73459.111000000004</v>
       </c>
-      <c r="Q36" s="11" t="s">
+      <c r="Q36" s="6" t="s">
         <v>37</v>
       </c>
       <c r="R36" s="6"/>
-      <c r="S36" s="23" t="s">
+      <c r="S36" s="19" t="s">
         <v>7</v>
       </c>
       <c r="T36" s="10">
@@ -3824,31 +3805,31 @@
       </c>
     </row>
     <row r="37">
-      <c r="G37" s="15" t="s">
+      <c r="G37" s="13" t="s">
         <v>38</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" t="s">
         <v>16</v>
       </c>
-      <c r="J37" s="13">
+      <c r="J37" s="12">
         <v>271.03300000000002</v>
       </c>
-      <c r="L37" s="26" t="s">
+      <c r="L37" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M37" s="6"/>
-      <c r="N37" s="27" t="s">
+      <c r="N37" s="23" t="s">
         <v>16</v>
       </c>
       <c r="O37" s="10">
         <v>271.03300000000002</v>
       </c>
-      <c r="Q37" s="26" t="s">
+      <c r="Q37" s="22" t="s">
         <v>38</v>
       </c>
       <c r="R37" s="6"/>
-      <c r="S37" s="27" t="s">
+      <c r="S37" s="23" t="s">
         <v>16</v>
       </c>
       <c r="T37" s="10">
@@ -3856,31 +3837,31 @@
       </c>
     </row>
     <row r="38">
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" t="s">
         <v>19</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="12">
         <v>130.685</v>
       </c>
-      <c r="L38" s="15" t="s">
+      <c r="L38" s="13" t="s">
         <v>18</v>
       </c>
       <c r="M38" s="6"/>
-      <c r="N38" s="23" t="s">
+      <c r="N38" s="19" t="s">
         <v>19</v>
       </c>
       <c r="O38" s="10">
         <v>130.68600000000001</v>
       </c>
-      <c r="Q38" s="15" t="s">
+      <c r="Q38" s="13" t="s">
         <v>18</v>
       </c>
       <c r="R38" s="6"/>
-      <c r="S38" s="23" t="s">
+      <c r="S38" s="19" t="s">
         <v>19</v>
       </c>
       <c r="T38" s="10">
@@ -3893,12 +3874,12 @@
       <c r="I39" t="s">
         <v>20</v>
       </c>
-      <c r="J39" s="13">
+      <c r="J39" s="12">
         <v>0.83699999999999997</v>
       </c>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
-      <c r="N39" s="27" t="s">
+      <c r="N39" s="23" t="s">
         <v>20</v>
       </c>
       <c r="O39" s="10">
@@ -3906,7 +3887,7 @@
       </c>
       <c r="Q39" s="6"/>
       <c r="R39" s="6"/>
-      <c r="S39" s="27" t="s">
+      <c r="S39" s="23" t="s">
         <v>20</v>
       </c>
       <c r="T39" s="10">
@@ -3919,12 +3900,12 @@
       <c r="I40" t="s">
         <v>21</v>
       </c>
-      <c r="J40" s="13">
+      <c r="J40" s="12">
         <v>0.68200000000000005</v>
       </c>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
-      <c r="N40" s="23" t="s">
+      <c r="N40" s="19" t="s">
         <v>21</v>
       </c>
       <c r="O40" s="10">
@@ -3932,7 +3913,7 @@
       </c>
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
-      <c r="S40" s="23" t="s">
+      <c r="S40" s="19" t="s">
         <v>21</v>
       </c>
       <c r="T40" s="10">
@@ -3945,23 +3926,23 @@
       <c r="I41" t="s">
         <v>22</v>
       </c>
-      <c r="J41" s="19">
+      <c r="J41" s="17">
         <v>1.1699999999999999</v>
       </c>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
-      <c r="N41" s="27" t="s">
+      <c r="N41" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="O41" s="18">
+      <c r="O41" s="16">
         <v>2.2000000000000002</v>
       </c>
       <c r="Q41" s="6"/>
       <c r="R41" s="6"/>
-      <c r="S41" s="27" t="s">
+      <c r="S41" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="T41" s="18">
+      <c r="T41" s="16">
         <v>1.8</v>
       </c>
     </row>
@@ -4033,7 +4014,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="100" workbookViewId="0">
       <selection activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -4075,14 +4056,14 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" ht="15.75">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="6"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="12">
         <v>73363.759000000005</v>
       </c>
       <c r="H4" s="6" t="s">
@@ -4099,43 +4080,43 @@
       </c>
     </row>
     <row r="5" ht="15.75">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="12">
         <v>270.85700000000003</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="20">
         <v>4</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="21">
         <v>68</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="21">
         <v>1.1899999999999999</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K5" s="21">
         <v>0.83999999999999997</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="12">
         <v>130.572</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="14">
         <v>4.0999999999999996</v>
       </c>
       <c r="I6" s="6">
@@ -4150,35 +4131,35 @@
     </row>
     <row r="7">
       <c r="D7" s="6"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="12">
         <v>0.83799999999999997</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="14">
         <v>4.2000000000000002</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="6">
         <v>68</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="6">
         <v>1.8999999999999999</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="6">
         <v>0.52000000000000002</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="12">
         <v>0.68200000000000005</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="14">
         <v>4.2999999999999998</v>
       </c>
       <c r="I8" s="6">
@@ -4194,13 +4175,13 @@
     <row r="9">
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>1.1899999999999999</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="14">
         <v>4.4000000000000004</v>
       </c>
       <c r="I9" s="6">
@@ -4215,7 +4196,6 @@
     </row>
     <row r="10"/>
     <row r="11" ht="15.75">
-      <c r="C11"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
         <v>5</v>
@@ -4223,11 +4203,11 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" ht="15.75">
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="10">
@@ -4235,11 +4215,11 @@
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="23" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="10">
@@ -4247,11 +4227,11 @@
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="10">
@@ -4261,7 +4241,7 @@
     <row r="15">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="23" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="10">
@@ -4271,7 +4251,7 @@
     <row r="16">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="10">
@@ -4281,17 +4261,16 @@
     <row r="17">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="16">
         <v>1.8</v>
       </c>
     </row>
     <row r="18"/>
     <row r="19">
-      <c r="B19" s="15"/>
-      <c r="C19"/>
+      <c r="B19" s="13"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6" t="s">
         <v>5</v>
@@ -4299,12 +4278,12 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20">
-      <c r="B20" s="15"/>
-      <c r="C20" s="11" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F20" s="10">
@@ -4312,11 +4291,11 @@
       </c>
     </row>
     <row r="21">
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="23" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="10">
@@ -4324,11 +4303,11 @@
       </c>
     </row>
     <row r="22">
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="10">
@@ -4338,7 +4317,7 @@
     <row r="23">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="23" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="10">
@@ -4348,7 +4327,7 @@
     <row r="24">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="10">
@@ -4356,25 +4335,25 @@
       </c>
     </row>
     <row r="25">
-      <c r="B25" s="15"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="16">
         <v>1.8999999999999999</v>
       </c>
     </row>
     <row r="26" ht="15.75">
-      <c r="B26" s="15"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="20"/>
+      <c r="E26" s="18"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" ht="15.75">
-      <c r="B27" s="15"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="9" t="s">
@@ -4383,12 +4362,12 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28">
-      <c r="B28" s="15"/>
-      <c r="C28" s="11" t="s">
+      <c r="B28" s="13"/>
+      <c r="C28" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="19" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="10">
@@ -4396,11 +4375,11 @@
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="22" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="27" t="s">
+      <c r="E29" s="23" t="s">
         <v>16</v>
       </c>
       <c r="F29" s="10">
@@ -4408,11 +4387,11 @@
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>42</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F30" s="10">
@@ -4422,7 +4401,7 @@
     <row r="31">
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="23" t="s">
         <v>20</v>
       </c>
       <c r="F31" s="10">
@@ -4430,10 +4409,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="15"/>
+      <c r="B32" s="13"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="19" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="10">
@@ -4441,25 +4420,25 @@
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="15"/>
+      <c r="B33" s="13"/>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="16">
         <v>1.7</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="15"/>
+      <c r="B34" s="13"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
     <row r="35">
-      <c r="B35" s="15"/>
+      <c r="B35" s="13"/>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="9" t="s">
@@ -4468,38 +4447,38 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36">
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="10">
         <v>73370.963000000003</v>
       </c>
     </row>
     <row r="37">
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="10">
         <v>270.87099999999998</v>
       </c>
     </row>
     <row r="38">
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>43</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="10">
         <v>130.58099999999999</v>
       </c>
     </row>
@@ -4509,7 +4488,7 @@
       <c r="E39" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="10">
         <v>0.83699999999999997</v>
       </c>
     </row>
@@ -4519,7 +4498,7 @@
       <c r="E40" t="s">
         <v>21</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F40" s="10">
         <v>0.68200000000000005</v>
       </c>
     </row>
@@ -4529,7 +4508,7 @@
       <c r="E41" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="16">
         <v>1.75</v>
       </c>
     </row>

</xml_diff>